<commit_message>
added support for Computes/HSN-bmcs/VizNodes/LoginNodes/pdu during config generation
</commit_message>
<xml_diff>
--- a/tests/data/Architecture_Golden_Config_Dellanox.xlsx
+++ b/tests/data/Architecture_Golden_Config_Dellanox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasbates/canu-container/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7923D-235C-7246-A7FA-72DD76CB9529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CECDA6-2902-AB49-BEA4-5CF8DF5F2D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="1640" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="79000" yWindow="-7960" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="SWITCH_TO_SWITCH" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="55">
   <si>
     <t>Source</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>sw-smn01</t>
+  </si>
+  <si>
+    <t>onboard</t>
   </si>
 </sst>
 </file>
@@ -2518,6 +2521,9 @@
       <c r="L24" t="s">
         <v>45</v>
       </c>
+      <c r="M24" t="s">
+        <v>54</v>
+      </c>
       <c r="O24">
         <v>1</v>
       </c>
@@ -2544,6 +2550,9 @@
       <c r="L25" t="s">
         <v>47</v>
       </c>
+      <c r="M25" t="s">
+        <v>54</v>
+      </c>
       <c r="O25">
         <v>1</v>
       </c>
@@ -2570,6 +2579,9 @@
       <c r="L26" t="s">
         <v>49</v>
       </c>
+      <c r="M26" t="s">
+        <v>54</v>
+      </c>
       <c r="O26">
         <v>1</v>
       </c>
@@ -2595,6 +2607,9 @@
       </c>
       <c r="L27" t="s">
         <v>51</v>
+      </c>
+      <c r="M27" t="s">
+        <v>54</v>
       </c>
       <c r="O27">
         <v>1</v>

</xml_diff>

<commit_message>
Casmnet 896 bgp support (#49)
* added Aruba BGP support

* update aruba tests for BGP

* added Mellanox BGP support

* update mellanox template/tests

* update readme

* added support for Computes/HSN-bmcs/VizNodes/LoginNodes/pdu during config generation

* update cray-network-architecture.yaml

Co-authored-by: lukebates123 <lucas.bates@hpe.com>
</commit_message>
<xml_diff>
--- a/tests/data/Architecture_Golden_Config_Dellanox.xlsx
+++ b/tests/data/Architecture_Golden_Config_Dellanox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lucasbates/canu-container/canu/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E7923D-235C-7246-A7FA-72DD76CB9529}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50CECDA6-2902-AB49-BEA4-5CF8DF5F2D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5200" yWindow="1640" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
+    <workbookView xWindow="79000" yWindow="-7960" windowWidth="28040" windowHeight="17040" activeTab="3" xr2:uid="{4E3EDB71-9423-764F-AB16-D8E153A84166}"/>
   </bookViews>
   <sheets>
     <sheet name="SWITCH_TO_SWITCH" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="55">
   <si>
     <t>Source</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>sw-smn01</t>
+  </si>
+  <si>
+    <t>onboard</t>
   </si>
 </sst>
 </file>
@@ -2518,6 +2521,9 @@
       <c r="L24" t="s">
         <v>45</v>
       </c>
+      <c r="M24" t="s">
+        <v>54</v>
+      </c>
       <c r="O24">
         <v>1</v>
       </c>
@@ -2544,6 +2550,9 @@
       <c r="L25" t="s">
         <v>47</v>
       </c>
+      <c r="M25" t="s">
+        <v>54</v>
+      </c>
       <c r="O25">
         <v>1</v>
       </c>
@@ -2570,6 +2579,9 @@
       <c r="L26" t="s">
         <v>49</v>
       </c>
+      <c r="M26" t="s">
+        <v>54</v>
+      </c>
       <c r="O26">
         <v>1</v>
       </c>
@@ -2595,6 +2607,9 @@
       </c>
       <c r="L27" t="s">
         <v>51</v>
+      </c>
+      <c r="M27" t="s">
+        <v>54</v>
       </c>
       <c r="O27">
         <v>1</v>

</xml_diff>